<commit_message>
prépa - traitement données erié élèves
mise en forme du database et du rmd pour générer les graphs emo et cps (experimental)
</commit_message>
<xml_diff>
--- a/hlm2021_nb/erie.xlsx
+++ b/hlm2021_nb/erie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbr/Documents/GitHub/r-projects/hlm2021_nb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9EE47F-78EE-344B-89F7-FDE1F05DF754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A35DAC-016E-734A-BDAF-22DC5C8382C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{B856B97F-0C03-1347-9D24-56AEBEBD8981}"/>
+    <workbookView xWindow="10360" yWindow="2740" windowWidth="28040" windowHeight="17440" xr2:uid="{B856B97F-0C03-1347-9D24-56AEBEBD8981}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>classe</t>
-  </si>
-  <si>
-    <t>id_enfant</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>age</t>
   </si>
@@ -51,41 +45,128 @@
     <t>date_mesure</t>
   </si>
   <si>
-    <t>emo3_1</t>
-  </si>
-  <si>
-    <t>emo3_2</t>
-  </si>
-  <si>
-    <t>emo3_3</t>
-  </si>
-  <si>
-    <t>cps2_1</t>
-  </si>
-  <si>
-    <t>cps2_2</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>code</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>emo5_1</t>
+  </si>
+  <si>
+    <t>emo5_2</t>
+  </si>
+  <si>
+    <t>emo5_3</t>
+  </si>
+  <si>
+    <t>emo5_4</t>
+  </si>
+  <si>
+    <t>emo5_5</t>
+  </si>
+  <si>
+    <t>cps26_1</t>
+  </si>
+  <si>
+    <t>cps26_2</t>
+  </si>
+  <si>
+    <t>cps26_3</t>
+  </si>
+  <si>
+    <t>cps26_4</t>
+  </si>
+  <si>
+    <t>cps26_5</t>
+  </si>
+  <si>
+    <t>cps26_6</t>
+  </si>
+  <si>
+    <t>cps26_7</t>
+  </si>
+  <si>
+    <t>cps26_8</t>
+  </si>
+  <si>
+    <t>cps26_9</t>
+  </si>
+  <si>
+    <t>cps26_10</t>
+  </si>
+  <si>
+    <t>cps26_11</t>
+  </si>
+  <si>
+    <t>cps26_12</t>
+  </si>
+  <si>
+    <t>cps26_13</t>
+  </si>
+  <si>
+    <t>cps26_14</t>
+  </si>
+  <si>
+    <t>cps26_15</t>
+  </si>
+  <si>
+    <t>cps26_16</t>
+  </si>
+  <si>
+    <t>cps26_17</t>
+  </si>
+  <si>
+    <t>cps26_18</t>
+  </si>
+  <si>
+    <t>cps26_19</t>
+  </si>
+  <si>
+    <t>cps26_20</t>
+  </si>
+  <si>
+    <t>cps26_21</t>
+  </si>
+  <si>
+    <t>cps26_22</t>
+  </si>
+  <si>
+    <t>cps26_23</t>
+  </si>
+  <si>
+    <t>cps26_24</t>
+  </si>
+  <si>
+    <t>cps26_25</t>
+  </si>
+  <si>
+    <t>cps26_26</t>
+  </si>
+  <si>
+    <t>123a15</t>
+  </si>
+  <si>
+    <t>123a25</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,6 +210,140 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657679</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>45357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>589643</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>11339</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC6C399C-E363-0441-9526-3940D412D995}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4796518" y="1474107"/>
+          <a:ext cx="2415268" cy="3027589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>code : code</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> de la classe au temps mesuré (exemple : 123a25)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>id : code unique pour reconnaitre l'enfant entre le temps et le temps 2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>age : age</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> sexe : sexe g ou f</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>emo : .... scores emo</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>cps : ... scores cps</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>date_mesure : date de la mesure</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>par : erié</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,143 +643,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B7F297-EB78-0248-B58D-84709A55E108}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:AK4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>44359</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <v>5</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2">
+        <v>5</v>
+      </c>
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <v>5</v>
+      </c>
+      <c r="X2">
+        <v>5</v>
+      </c>
+      <c r="Y2">
+        <v>5</v>
+      </c>
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
+        <v>5</v>
+      </c>
+      <c r="AB2">
+        <v>5</v>
+      </c>
+      <c r="AC2">
+        <v>5</v>
+      </c>
+      <c r="AD2">
+        <v>5</v>
+      </c>
+      <c r="AE2">
+        <v>5</v>
+      </c>
+      <c r="AF2">
+        <v>5</v>
+      </c>
+      <c r="AG2">
+        <v>5</v>
+      </c>
+      <c r="AH2">
+        <v>5</v>
+      </c>
+      <c r="AI2">
+        <v>5</v>
+      </c>
+      <c r="AJ2">
+        <v>5</v>
+      </c>
+      <c r="AK2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>5</v>
+      </c>
+      <c r="V3">
+        <v>5</v>
+      </c>
+      <c r="W3">
+        <v>5</v>
+      </c>
+      <c r="X3">
+        <v>5</v>
+      </c>
+      <c r="Y3">
+        <v>5</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>5</v>
+      </c>
+      <c r="AB3">
+        <v>5</v>
+      </c>
+      <c r="AC3">
+        <v>5</v>
+      </c>
+      <c r="AD3">
+        <v>5</v>
+      </c>
+      <c r="AE3">
+        <v>5</v>
+      </c>
+      <c r="AF3">
+        <v>5</v>
+      </c>
+      <c r="AG3">
+        <v>5</v>
+      </c>
+      <c r="AH3">
+        <v>5</v>
+      </c>
+      <c r="AI3">
+        <v>5</v>
+      </c>
+      <c r="AJ3">
+        <v>5</v>
+      </c>
+      <c r="AK3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1">
-        <v>44359</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1">
-        <v>44359</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4">
+        <v>5</v>
+      </c>
+      <c r="U4">
+        <v>5</v>
+      </c>
+      <c r="V4">
+        <v>5</v>
+      </c>
+      <c r="W4">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>5</v>
+      </c>
+      <c r="Y4">
+        <v>5</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+      <c r="AA4">
+        <v>5</v>
+      </c>
+      <c r="AB4">
+        <v>5</v>
+      </c>
+      <c r="AC4">
+        <v>5</v>
+      </c>
+      <c r="AD4">
+        <v>5</v>
+      </c>
+      <c r="AE4">
+        <v>5</v>
+      </c>
+      <c r="AF4">
+        <v>5</v>
+      </c>
+      <c r="AG4">
+        <v>5</v>
+      </c>
+      <c r="AH4">
+        <v>5</v>
+      </c>
+      <c r="AI4">
+        <v>5</v>
+      </c>
+      <c r="AJ4">
+        <v>5</v>
+      </c>
+      <c r="AK4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>